<commit_message>
add a home page
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elona/Desktop/UNESCO/G20 work/tpaf-visualizer/public/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elona/Desktop/UNESCO/G20 work/policy-tool/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F30882-A21D-4C44-9C70-F1B62DDB8EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18D144E-A7E1-624B-9159-B452675AE91A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="4" xr2:uid="{D9812107-478A-4822-AECD-ADE43880D8CA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{D9812107-478A-4822-AECD-ADE43880D8CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Enabling Infrastructure" sheetId="1" r:id="rId1"/>
@@ -166,7 +166,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="227">
   <si>
     <t>Phases of the Policy Option
 (relevance/goal)</t>
@@ -2050,9 +2050,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Roll out public and private sector partnerships for AI apprenticeships , internships; and tailored skills-building programs </t>
-  </si>
-  <si>
     <t>Conduct scoping studies and foresight assessments</t>
   </si>
   <si>
@@ -2848,6 +2845,9 @@
   </si>
   <si>
     <t>Policy Implementation</t>
+  </si>
+  <si>
+    <t>Lorem Ipsum is simply dummy text of the printing and typesetting industry.</t>
   </si>
 </sst>
 </file>
@@ -4256,7 +4256,7 @@
     </row>
     <row r="2" spans="1:5" ht="72.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A2" s="98" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B2" s="38" t="s">
         <v>5</v>
@@ -4341,7 +4341,7 @@
     </row>
     <row r="9" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="104" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B9" s="61" t="s">
         <v>22</v>
@@ -4450,7 +4450,7 @@
     </row>
     <row r="18" spans="1:5" ht="288" x14ac:dyDescent="0.2">
       <c r="A18" s="108" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B18" s="56" t="s">
         <v>44</v>
@@ -4606,7 +4606,7 @@
     </row>
     <row r="2" spans="1:5" ht="80" x14ac:dyDescent="0.2">
       <c r="A2" s="118" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B2" s="121" t="s">
         <v>60</v>
@@ -4668,7 +4668,7 @@
     </row>
     <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="118" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B8" s="116" t="s">
         <v>72</v>
@@ -4720,7 +4720,7 @@
     </row>
     <row r="13" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="118" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B13" s="116" t="s">
         <v>82</v>
@@ -4845,9 +4845,9 @@
   </sheetPr>
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A8"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4879,7 +4879,7 @@
     </row>
     <row r="2" spans="1:5" ht="335" x14ac:dyDescent="0.2">
       <c r="A2" s="122" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>102</v>
@@ -4956,7 +4956,7 @@
     </row>
     <row r="9" spans="1:5" ht="112" x14ac:dyDescent="0.2">
       <c r="A9" s="123" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>115</v>
@@ -5011,7 +5011,7 @@
     </row>
     <row r="14" spans="1:5" ht="176" x14ac:dyDescent="0.2">
       <c r="A14" s="122" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B14" s="128" t="s">
         <v>124</v>
@@ -5050,11 +5050,15 @@
       <c r="A17" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="B17" s="78"/>
+      <c r="B17" s="78" t="s">
+        <v>226</v>
+      </c>
       <c r="C17" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="D17" s="79"/>
+        <v>226</v>
+      </c>
+      <c r="D17" s="79" t="s">
+        <v>226</v>
+      </c>
       <c r="E17" s="41"/>
       <c r="F17" s="41"/>
     </row>
@@ -5130,16 +5134,16 @@
     </row>
     <row r="2" spans="1:5" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="143" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B2" s="156" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" s="158" t="s">
         <v>133</v>
       </c>
-      <c r="C2" s="158" t="s">
+      <c r="D2" s="19" t="s">
         <v>134</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="98.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5147,67 +5151,67 @@
       <c r="B3" s="157"/>
       <c r="C3" s="112"/>
       <c r="D3" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="145"/>
       <c r="B4" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="51" t="s">
         <v>137</v>
-      </c>
-      <c r="C4" s="51" t="s">
-        <v>138</v>
       </c>
       <c r="D4" s="19"/>
     </row>
     <row r="5" spans="1:5" ht="154.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="146"/>
       <c r="B5" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="D5" s="87" t="s">
         <v>140</v>
-      </c>
-      <c r="D5" s="87" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="42" customFormat="1" ht="153" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="149" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B6" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="80" t="s">
         <v>142</v>
       </c>
-      <c r="C6" s="80" t="s">
+      <c r="D6" s="19" t="s">
         <v>143</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="166.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="150"/>
       <c r="B7" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" s="45" t="s">
         <v>145</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="D7" s="86" t="s">
         <v>146</v>
-      </c>
-      <c r="D7" s="86" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="145" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="151"/>
       <c r="B8" s="148" t="s">
+        <v>147</v>
+      </c>
+      <c r="C8" s="159" t="s">
         <v>148</v>
       </c>
-      <c r="C8" s="159" t="s">
+      <c r="D8" s="20" t="s">
         <v>149</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="181.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -5215,19 +5219,19 @@
       <c r="B9" s="148"/>
       <c r="C9" s="160"/>
       <c r="D9" s="19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="115.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="150"/>
       <c r="B10" s="153" t="s">
+        <v>151</v>
+      </c>
+      <c r="C10" s="161" t="s">
         <v>152</v>
       </c>
-      <c r="C10" s="161" t="s">
+      <c r="D10" s="89" t="s">
         <v>153</v>
-      </c>
-      <c r="D10" s="89" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="115.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -5244,13 +5248,13 @@
     </row>
     <row r="13" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="147" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B13" s="148" t="s">
+        <v>154</v>
+      </c>
+      <c r="C13" s="52" t="s">
         <v>155</v>
-      </c>
-      <c r="C13" s="52" t="s">
-        <v>156</v>
       </c>
       <c r="D13" s="141"/>
     </row>
@@ -5258,7 +5262,7 @@
       <c r="A14" s="144"/>
       <c r="B14" s="148"/>
       <c r="C14" s="44" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D14" s="142"/>
     </row>
@@ -5266,59 +5270,59 @@
       <c r="A15" s="144"/>
       <c r="B15" s="148"/>
       <c r="C15" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="D15" s="91" t="s">
         <v>158</v>
-      </c>
-      <c r="D15" s="91" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="144"/>
       <c r="B16" s="164" t="s">
+        <v>159</v>
+      </c>
+      <c r="C16" s="45" t="s">
         <v>160</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="D16" s="18" t="s">
         <v>161</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="144"/>
       <c r="B17" s="165"/>
       <c r="C17" s="43" t="s">
+        <v>162</v>
+      </c>
+      <c r="D17" s="92" t="s">
         <v>163</v>
-      </c>
-      <c r="D17" s="92" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="144"/>
       <c r="B18" s="166"/>
       <c r="C18" s="81" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D18" s="19"/>
     </row>
     <row r="19" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="144"/>
       <c r="B19" s="138" t="s">
+        <v>165</v>
+      </c>
+      <c r="C19" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="D19" s="92" t="s">
         <v>167</v>
-      </c>
-      <c r="D19" s="92" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="144"/>
       <c r="B20" s="139"/>
       <c r="C20" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D20" s="93"/>
     </row>
@@ -5326,7 +5330,7 @@
       <c r="A21" s="144"/>
       <c r="B21" s="140"/>
       <c r="C21" s="75" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D21" s="93"/>
     </row>
@@ -5335,30 +5339,30 @@
         <v>56</v>
       </c>
       <c r="B22" s="82" t="s">
+        <v>170</v>
+      </c>
+      <c r="C22" s="83" t="s">
         <v>171</v>
-      </c>
-      <c r="C22" s="83" t="s">
-        <v>172</v>
       </c>
       <c r="D22" s="94"/>
     </row>
     <row r="23" spans="1:4" ht="108.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="144"/>
       <c r="B23" s="82" t="s">
+        <v>172</v>
+      </c>
+      <c r="C23" s="83" t="s">
         <v>173</v>
-      </c>
-      <c r="C23" s="83" t="s">
-        <v>174</v>
       </c>
       <c r="D23" s="95"/>
     </row>
     <row r="24" spans="1:4" ht="111.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="146"/>
       <c r="B24" s="84" t="s">
+        <v>174</v>
+      </c>
+      <c r="C24" s="85" t="s">
         <v>175</v>
-      </c>
-      <c r="C24" s="85" t="s">
-        <v>176</v>
       </c>
       <c r="D24" s="96"/>
     </row>
@@ -5392,7 +5396,7 @@
   </sheetPr>
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
+    <sheetView zoomScale="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13:A16"/>
@@ -5428,153 +5432,153 @@
     </row>
     <row r="2" spans="1:5" ht="387.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="167" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B2" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="C2" s="37" t="s">
         <v>177</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="D2" s="38" t="s">
         <v>178</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="E2" s="28" t="s">
         <v>179</v>
-      </c>
-      <c r="E2" s="28" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="186" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="168"/>
       <c r="B3" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" s="38" t="s">
         <v>181</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="D3" s="29" t="s">
         <v>182</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="E3" s="39" t="s">
         <v>183</v>
-      </c>
-      <c r="E3" s="39" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="198" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="168"/>
       <c r="B4" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="C4" s="38" t="s">
         <v>185</v>
-      </c>
-      <c r="C4" s="38" t="s">
-        <v>186</v>
       </c>
       <c r="D4" s="40"/>
       <c r="E4" s="28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="171" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B5" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="C5" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="D5" s="169" t="s">
         <v>189</v>
       </c>
-      <c r="D5" s="169" t="s">
+      <c r="E5" s="28" t="s">
         <v>190</v>
-      </c>
-      <c r="E5" s="28" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="171"/>
       <c r="B6" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="C6" s="38" t="s">
         <v>192</v>
-      </c>
-      <c r="C6" s="38" t="s">
-        <v>193</v>
       </c>
       <c r="D6" s="169"/>
       <c r="E6" s="28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="267.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="171"/>
       <c r="B7" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="C7" s="38" t="s">
         <v>195</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>196</v>
       </c>
       <c r="D7" s="38"/>
       <c r="E7" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="224" x14ac:dyDescent="0.2">
       <c r="A8" s="171"/>
       <c r="B8" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="C8" s="38" t="s">
         <v>198</v>
-      </c>
-      <c r="C8" s="38" t="s">
-        <v>199</v>
       </c>
       <c r="D8" s="38"/>
       <c r="E8" s="28"/>
     </row>
     <row r="9" spans="1:5" ht="96" x14ac:dyDescent="0.2">
       <c r="A9" s="167" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B9" s="170" t="s">
+        <v>199</v>
+      </c>
+      <c r="C9" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="D9" s="38" t="s">
         <v>201</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="E9" s="28" t="s">
         <v>202</v>
-      </c>
-      <c r="E9" s="28" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A10" s="171"/>
       <c r="B10" s="170"/>
       <c r="C10" s="38" t="s">
+        <v>203</v>
+      </c>
+      <c r="D10" s="38" t="s">
         <v>204</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="E10" s="28" t="s">
         <v>205</v>
-      </c>
-      <c r="E10" s="28" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="112" x14ac:dyDescent="0.2">
       <c r="A11" s="171"/>
       <c r="B11" s="28" t="s">
+        <v>206</v>
+      </c>
+      <c r="C11" s="38" t="s">
         <v>207</v>
-      </c>
-      <c r="C11" s="38" t="s">
-        <v>208</v>
       </c>
       <c r="D11" s="38"/>
       <c r="E11" s="28" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="288" x14ac:dyDescent="0.2">
       <c r="A12" s="171"/>
       <c r="B12" s="28" t="s">
+        <v>209</v>
+      </c>
+      <c r="C12" s="38" t="s">
         <v>210</v>
-      </c>
-      <c r="C12" s="38" t="s">
-        <v>211</v>
       </c>
       <c r="D12" s="38"/>
       <c r="E12" s="28"/>
@@ -5584,53 +5588,53 @@
         <v>56</v>
       </c>
       <c r="B13" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="C13" s="38" t="s">
         <v>212</v>
-      </c>
-      <c r="C13" s="38" t="s">
-        <v>213</v>
       </c>
       <c r="D13" s="38"/>
       <c r="E13" s="28" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="168"/>
       <c r="B14" s="28" t="s">
+        <v>214</v>
+      </c>
+      <c r="C14" s="38" t="s">
         <v>215</v>
-      </c>
-      <c r="C14" s="38" t="s">
-        <v>216</v>
       </c>
       <c r="D14" s="38"/>
       <c r="E14" s="28" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="168"/>
       <c r="B15" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="C15" s="38" t="s">
         <v>218</v>
-      </c>
-      <c r="C15" s="38" t="s">
-        <v>219</v>
       </c>
       <c r="D15" s="38"/>
       <c r="E15" s="28" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="168"/>
       <c r="B16" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="C16" s="38" t="s">
         <v>221</v>
-      </c>
-      <c r="C16" s="38" t="s">
-        <v>222</v>
       </c>
       <c r="D16" s="38"/>
       <c r="E16" s="28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>